<commit_message>
add models_to_exclude to Template and pipeline
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>retention_time_estimate</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Only if pre_filtering was set to "True" (see settings).</t>
+  </si>
+  <si>
+    <t>models_to_exclude_from_selection</t>
   </si>
 </sst>
 </file>
@@ -785,7 +788,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +812,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +877,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,10 +888,11 @@
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -899,6 +903,9 @@
         <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>